<commit_message>
left overs of modernisation of features, documenting modernisation
</commit_message>
<xml_diff>
--- a/docs/DataDic.xlsx
+++ b/docs/DataDic.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="125">
   <si>
     <t xml:space="preserve">Column Name</t>
   </si>
@@ -209,127 +209,193 @@
     <t xml:space="preserve">Target variable</t>
   </si>
   <si>
-    <t xml:space="preserve">New Column</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description (Modern Context)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Why It Increases Hiring Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">daily_watch_minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average minutes spent daily on the app</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measures engagement depth</t>
+    <t xml:space="preserve">New Column Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why It Matters / Increases Hiring Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique identifier assigned to each customer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensures accurate tracking and merging of customer-level data, demonstrating data management skills.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender of the customer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helps analyze demographic trends affecting churn and customer behavior.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">months_subscribed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total number of months the customer has been subscribed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strong churn predictor and useful for retention modeling and cohort analysis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">streaming_quality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferred streaming quality selected by the customer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helps assess user preferences and link quality tiers to revenue and churn risk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subscription_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of subscription plan chosen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key segmentation feature for predicting churn and understanding plan profitability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">payment_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode of payment used by the customer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useful for identifying payment-related churn patterns and operational bottlenecks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthly_plan_cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly cost of the subscription plan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows modeling of price sensitivity and revenue optimization strategies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total revenue collected from the customer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core feature for CLTV modeling and high-value customer identification.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subscription_canceled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicates if the subscription was canceled (1 = Yes, 0 = No).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target variable for churn prediction and retention intervention strategies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app_usage_hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average daily app usage hours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Behavior-based predictor of engagement and churn probability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last30d_usage_hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total app usage in the last 30 days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Captures short-term engagement trends critical for churn modeling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer_rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer satisfaction rating on a 1–5 scale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Links customer sentiment to churn, enhancing predictive model performance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">promo_email_clicks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of promotional emails clicked.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measures marketing responsiveness and helps build retention/upsell strategies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">device_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary device type used by the customer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Useful for UX optimization and device-based user behavior segmentation.</t>
   </si>
   <si>
     <t xml:space="preserve">num_profiles</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of user profiles under the account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common for OTT subscriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">device_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile / TV / Laptop / Multiple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Industry metric for churn risk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferred_genre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drama/Action/Sports/Kids etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Highly used by streaming companies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ad_interactions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of ad clicks or skips</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relevant for ad-supported plans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app_rating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">float (1–5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User feedback rating inside app</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Survey-based churn indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">offer_redemption_count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How many promo codes redeemed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price-sensitive user indicator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">last_payment_success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Success / Failed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment failures cause churn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subscription_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free / Basic / Standard / Premium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTT-standard plan tiers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">viewing_hours_last_30d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total viewing hours in last month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retention measurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer_support_calls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total support escalations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High complaints → churn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">auto_renewal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto-renew enabled or not</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Critical churn factor</t>
+    <t xml:space="preserve">Number of profiles associated with the account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicates household engagement level and correlates with retention.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auto_renew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether auto-renewal is enabled (1 = Yes, 0 = No).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strong churn indicator and helpful feature for business rule–based models.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">support_tickets_last6m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of support tickets raised in the last 6 months.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helps measure friction points and improves service-related churn analysis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nps_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net Promoter Score given by the customer. (0-10 scale)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industry-standard loyalty metric that enriches churn and CLTV models.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_active_last30d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether customer was active in the last 30 days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A crucial recency feature that boosts predictive accuracy for churn models.</t>
   </si>
 </sst>
 </file>
@@ -339,11 +405,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -365,11 +432,20 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -414,16 +490,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -553,321 +641,322 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -887,197 +976,297 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="86.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="54.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>70</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>73</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="B5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="B6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>83</v>
       </c>
+      <c r="D7" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>86</v>
       </c>
+      <c r="C8" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>89</v>
       </c>
+      <c r="B9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="B10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="B11" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="B12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="B13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>102</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>